<commit_message>
Vollständige ausertung für 300 samples
</commit_message>
<xml_diff>
--- a/Auswertung.xlsx
+++ b/Auswertung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\StefanLap\BachelorKI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6D840B-4B8A-4C9C-A61C-3DFC227A3439}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE4879C-1434-41F1-B046-E4CDC308FB83}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11265" windowHeight="4485" xr2:uid="{22A6BE3B-3F0B-4EF0-96C7-C5709C02FF53}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="101">
   <si>
     <t>Classifier</t>
   </si>
@@ -40,9 +39,6 @@
     <t>Recall</t>
   </si>
   <si>
-    <t xml:space="preserve"> Gaussian Naive Bayes</t>
-  </si>
-  <si>
     <t>Content, Subject, Time, Attachment</t>
   </si>
   <si>
@@ -64,12 +60,6 @@
     <t>0.87</t>
   </si>
   <si>
-    <t>0.33 Splitrate</t>
-  </si>
-  <si>
-    <t>0.66 splitrate</t>
-  </si>
-  <si>
     <t>0.8</t>
   </si>
   <si>
@@ -79,9 +69,6 @@
     <t>82.0</t>
   </si>
   <si>
-    <t>0.98</t>
-  </si>
-  <si>
     <t>0.76</t>
   </si>
   <si>
@@ -91,12 +78,6 @@
     <t>0.88</t>
   </si>
   <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>0.90</t>
-  </si>
-  <si>
     <t>Anmerkung: Precision und Recall sind immer mit 0.5 split erfolgt</t>
   </si>
   <si>
@@ -133,9 +114,6 @@
     <t>84.3</t>
   </si>
   <si>
-    <t>81.49</t>
-  </si>
-  <si>
     <t>0.78</t>
   </si>
   <si>
@@ -148,15 +126,9 @@
     <t>0.57</t>
   </si>
   <si>
-    <t>0.52</t>
-  </si>
-  <si>
     <t>51.33</t>
   </si>
   <si>
-    <t>0.47</t>
-  </si>
-  <si>
     <t>0.55</t>
   </si>
   <si>
@@ -170,6 +142,192 @@
   </si>
   <si>
     <t>81.67</t>
+  </si>
+  <si>
+    <t>Gaussian NB</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>0.7</t>
+  </si>
+  <si>
+    <t>0.81</t>
+  </si>
+  <si>
+    <t>Specificity wenn value negativ gewertet wie oft war das korrekt</t>
+  </si>
+  <si>
+    <t>0.71</t>
+  </si>
+  <si>
+    <t>0.75</t>
+  </si>
+  <si>
+    <t>0.73</t>
+  </si>
+  <si>
+    <t>81.0</t>
+  </si>
+  <si>
+    <t>0.61</t>
+  </si>
+  <si>
+    <t>0.50</t>
+  </si>
+  <si>
+    <t>0.79</t>
+  </si>
+  <si>
+    <t>0.45</t>
+  </si>
+  <si>
+    <t>0.36</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>0.629</t>
+  </si>
+  <si>
+    <t>49.33</t>
+  </si>
+  <si>
+    <t>0.69</t>
+  </si>
+  <si>
+    <t>0.70</t>
+  </si>
+  <si>
+    <t>BernoulliNB</t>
+  </si>
+  <si>
+    <t>83.0</t>
+  </si>
+  <si>
+    <t>79.0</t>
+  </si>
+  <si>
+    <t>82.33</t>
+  </si>
+  <si>
+    <t>82.67</t>
+  </si>
+  <si>
+    <t>0.85</t>
+  </si>
+  <si>
+    <t>0.94</t>
+  </si>
+  <si>
+    <t>0.49</t>
+  </si>
+  <si>
+    <t>77.33</t>
+  </si>
+  <si>
+    <t>0.40</t>
+  </si>
+  <si>
+    <t>0.53</t>
+  </si>
+  <si>
+    <t>0.62</t>
+  </si>
+  <si>
+    <t>49.67</t>
+  </si>
+  <si>
+    <t>KNN(7 neighbors)</t>
+  </si>
+  <si>
+    <t>0.42</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>0.72</t>
+  </si>
+  <si>
+    <t>0.54</t>
+  </si>
+  <si>
+    <t>0.41</t>
+  </si>
+  <si>
+    <t>56.33</t>
+  </si>
+  <si>
+    <t>0.522</t>
+  </si>
+  <si>
+    <t>0.34</t>
+  </si>
+  <si>
+    <t>63.3</t>
+  </si>
+  <si>
+    <t>0.66</t>
+  </si>
+  <si>
+    <t>0.68</t>
+  </si>
+  <si>
+    <t>0.64</t>
+  </si>
+  <si>
+    <t>0.77</t>
+  </si>
+  <si>
+    <t>73.67</t>
+  </si>
+  <si>
+    <t>0.60</t>
+  </si>
+  <si>
+    <t>0.97</t>
+  </si>
+  <si>
+    <t>70.67</t>
+  </si>
+  <si>
+    <t>neuronal</t>
+  </si>
+  <si>
+    <t>0.80</t>
+  </si>
+  <si>
+    <t>20 Hiddenlayersize 400iterationen</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>0.58</t>
+  </si>
+  <si>
+    <t>84.6</t>
+  </si>
+  <si>
+    <t>83.6</t>
+  </si>
+  <si>
+    <t>84.0</t>
+  </si>
+  <si>
+    <t>83.67</t>
+  </si>
+  <si>
+    <t>84.1</t>
+  </si>
+  <si>
+    <t>80.8</t>
+  </si>
+  <si>
+    <t>0.65</t>
   </si>
 </sst>
 </file>
@@ -523,27 +681,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEEDE95E-D87B-482A-8A65-040653F3D525}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -552,33 +710,16 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="J1" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="K1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>300</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -586,31 +727,28 @@
         <v>300</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
       <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="J3" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -618,31 +756,28 @@
         <v>300</v>
       </c>
       <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>50</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J4" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -650,31 +785,28 @@
         <v>300</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" t="s">
         <v>46</v>
       </c>
-      <c r="F5" t="s">
-        <v>32</v>
-      </c>
       <c r="G5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="I5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="J5" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -682,31 +814,28 @@
         <v>300</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -714,31 +843,28 @@
         <v>300</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>33</v>
-      </c>
-      <c r="H7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -746,31 +872,28 @@
         <v>300</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E8">
         <v>84</v>
       </c>
       <c r="F8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G8" t="s">
-        <v>32</v>
-      </c>
-      <c r="H8" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="I8" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -778,31 +901,28 @@
         <v>300</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>81</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H9" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -810,216 +930,973 @@
         <v>300</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="G10" t="s">
-        <v>40</v>
-      </c>
-      <c r="H10" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="I10" t="s">
-        <v>42</v>
+        <v>75</v>
       </c>
       <c r="J10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>300</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>300</v>
       </c>
+      <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>41</v>
+      </c>
+      <c r="G12" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>300</v>
       </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>300</v>
       </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>300</v>
       </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>41</v>
+      </c>
+      <c r="G15" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>300</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" t="s">
+        <v>42</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
+      </c>
+      <c r="J16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>300</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" t="s">
+        <v>44</v>
+      </c>
+      <c r="G17" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" t="s">
+        <v>45</v>
+      </c>
+      <c r="J17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>300</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" t="s">
+        <v>60</v>
+      </c>
+      <c r="F18" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I18" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>300</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" t="s">
+        <v>53</v>
+      </c>
+      <c r="J19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>300</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>300</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" t="s">
+        <v>29</v>
+      </c>
+      <c r="I21" t="s">
+        <v>42</v>
+      </c>
+      <c r="J21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>300</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" t="s">
+        <v>11</v>
+      </c>
+      <c r="G22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>300</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23" t="s">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" t="s">
+        <v>42</v>
+      </c>
+      <c r="J23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>300</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" t="s">
+        <v>42</v>
+      </c>
+      <c r="J24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>300</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G25" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" t="s">
+        <v>42</v>
+      </c>
+      <c r="J25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>300</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>300</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" t="s">
+        <v>64</v>
+      </c>
+      <c r="I27" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>300</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" t="s">
+        <v>67</v>
+      </c>
+      <c r="I28" t="s">
+        <v>68</v>
+      </c>
+      <c r="J28" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>300</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>300</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>34</v>
+      </c>
+      <c r="G30" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" t="s">
+        <v>48</v>
+      </c>
+      <c r="J30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>300</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" t="s">
+        <v>56</v>
+      </c>
+      <c r="I31" t="s">
+        <v>75</v>
+      </c>
+      <c r="J31" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>300</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" t="s">
+        <v>78</v>
+      </c>
+      <c r="G32" t="s">
+        <v>27</v>
+      </c>
+      <c r="I32" t="s">
+        <v>32</v>
+      </c>
+      <c r="J32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>300</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" t="s">
+        <v>81</v>
+      </c>
+      <c r="G33" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>300</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>71</v>
+      </c>
+      <c r="C34" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" t="s">
+        <v>82</v>
+      </c>
+      <c r="G34" t="s">
+        <v>24</v>
+      </c>
+      <c r="I34" t="s">
+        <v>14</v>
+      </c>
+      <c r="J34" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>300</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D35" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F35" t="s">
+        <v>84</v>
+      </c>
+      <c r="G35" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>300</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>71</v>
+      </c>
+      <c r="C36" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" t="s">
+        <v>87</v>
+      </c>
+      <c r="I36" t="s">
+        <v>56</v>
+      </c>
+      <c r="J36" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>300</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D37" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" t="s">
+        <v>70</v>
+      </c>
+      <c r="F37" t="s">
+        <v>72</v>
+      </c>
+      <c r="G37" t="s">
+        <v>73</v>
+      </c>
+      <c r="I37" t="s">
+        <v>53</v>
+      </c>
+      <c r="J37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>300</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>300</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" t="s">
+        <v>8</v>
+      </c>
+      <c r="D39" t="s">
+        <v>4</v>
+      </c>
+      <c r="E39" t="s">
+        <v>95</v>
+      </c>
+      <c r="F39" t="s">
+        <v>90</v>
+      </c>
+      <c r="G39" t="s">
+        <v>26</v>
+      </c>
+      <c r="I39" t="s">
+        <v>26</v>
+      </c>
+      <c r="J39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>300</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" t="s">
+        <v>15</v>
+      </c>
+      <c r="E40" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" t="s">
+        <v>42</v>
+      </c>
+      <c r="I40" t="s">
+        <v>35</v>
+      </c>
+      <c r="J40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>300</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" t="s">
+        <v>96</v>
+      </c>
+      <c r="F41" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" t="s">
+        <v>26</v>
+      </c>
+      <c r="I41" t="s">
+        <v>26</v>
+      </c>
+      <c r="J41" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>300</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F42" t="s">
+        <v>11</v>
+      </c>
+      <c r="G42" t="s">
+        <v>30</v>
+      </c>
+      <c r="I42" t="s">
+        <v>27</v>
+      </c>
+      <c r="J42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>300</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" t="s">
+        <v>8</v>
+      </c>
+      <c r="D43" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" t="s">
+        <v>98</v>
+      </c>
+      <c r="F43" t="s">
+        <v>29</v>
+      </c>
+      <c r="G43" t="s">
+        <v>63</v>
+      </c>
+      <c r="I43" t="s">
+        <v>26</v>
+      </c>
+      <c r="J43" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>300</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" t="s">
+        <v>94</v>
+      </c>
+      <c r="F44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" t="s">
+        <v>26</v>
+      </c>
+      <c r="I44" t="s">
+        <v>26</v>
+      </c>
+      <c r="J44" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>300</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" t="s">
+        <v>8</v>
+      </c>
+      <c r="D45" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" t="s">
+        <v>57</v>
+      </c>
+      <c r="G45" t="s">
+        <v>10</v>
+      </c>
+      <c r="I45" t="s">
+        <v>84</v>
+      </c>
+      <c r="J45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>300</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>89</v>
+      </c>
+      <c r="C46" t="s">
+        <v>8</v>
+      </c>
+      <c r="D46" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" t="s">
+        <v>55</v>
+      </c>
+      <c r="F46" t="s">
+        <v>32</v>
+      </c>
+      <c r="G46" t="s">
+        <v>92</v>
+      </c>
+      <c r="I46" t="s">
+        <v>93</v>
+      </c>
+      <c r="J46" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>300</v>
+      </c>
+      <c r="B47" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>